<commit_message>
chore: :pencil2: Fix typos
</commit_message>
<xml_diff>
--- a/images/src/Tabellen.xlsx
+++ b/images/src/Tabellen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25407"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rene Hampölz\Desktop\CPE - Lastenlift-Steuerung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reneh\GitHub\htlweiz\HTL_Lastenlift\images\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6B6B06-6C66-441B-9186-C2F7E3FFEFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57364DFB-3A3E-485D-A986-2D6AF47D8130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{CA8AB77D-BEE3-4B25-8C58-C62C24F84226}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CA8AB77D-BEE3-4B25-8C58-C62C24F84226}"/>
   </bookViews>
   <sheets>
     <sheet name="Zustandstabelle" sheetId="1" r:id="rId1"/>
@@ -230,9 +230,6 @@
     <t>Q3 (Tür)</t>
   </si>
   <si>
-    <t>Tür blockiert, Auslösung durch lichtschranken</t>
-  </si>
-  <si>
     <t>Lift ist im 1. Stock angekommen</t>
   </si>
   <si>
@@ -269,12 +266,6 @@
     <t>sSendToS2</t>
   </si>
   <si>
-    <t>Lift fährt Rauf</t>
-  </si>
-  <si>
-    <t>Lift fährt Runter</t>
-  </si>
-  <si>
     <t>A6</t>
   </si>
   <si>
@@ -300,6 +291,15 @@
   </si>
   <si>
     <t>Tür im Lift schließen/öffnen (im 1. oder 2. Stock)</t>
+  </si>
+  <si>
+    <t>Tür blockiert, Auslösung durch Lichtschranken</t>
+  </si>
+  <si>
+    <t>Lift fährt rauf</t>
+  </si>
+  <si>
+    <t>Lift fährt runter</t>
   </si>
 </sst>
 </file>
@@ -831,7 +831,7 @@
   <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B2" sqref="B2:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +911,7 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -932,7 +932,7 @@
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C7" s="4"/>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -953,7 +953,7 @@
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>
@@ -974,7 +974,7 @@
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
       <c r="D9" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
         <v>27</v>
@@ -1005,7 +1005,7 @@
         <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I10" t="s">
         <v>44</v>
@@ -1014,16 +1014,16 @@
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
       <c r="D11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" t="s">
         <v>57</v>
@@ -1036,16 +1036,16 @@
       <c r="C12" s="4"/>
       <c r="D12" s="8"/>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
         <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I12" t="s">
         <v>44</v>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -1078,7 +1078,7 @@
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
@@ -1099,7 +1099,7 @@
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C15" s="5"/>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
         <v>31</v>
@@ -1120,7 +1120,7 @@
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
         <v>32</v>
@@ -1141,7 +1141,7 @@
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="5"/>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -1162,19 +1162,19 @@
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="5"/>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
         <v>44</v>
@@ -1183,19 +1183,19 @@
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="5"/>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" t="s">
         <v>80</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" t="s">
         <v>83</v>
-      </c>
-      <c r="G19" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" t="s">
-        <v>86</v>
       </c>
       <c r="I19" t="s">
         <v>44</v>
@@ -1212,5 +1212,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>